<commit_message>
So much done, it is a-fucking-mazing
</commit_message>
<xml_diff>
--- a/addresses.xlsx
+++ b/addresses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>line1</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>26772 Calle Maria</t>
+  </si>
+  <si>
+    <t>Capistrano Beach</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>us</t>
   </si>
 </sst>
 </file>
@@ -380,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,6 +446,23 @@
         <v>98311</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>92624</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>